<commit_message>
Cosco and ONE search and dictionary population completed
</commit_message>
<xml_diff>
--- a/Shipping Excel Sheet.xlsx
+++ b/Shipping Excel Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmattison\Desktop\ecopax-shipping-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00393AF7-1693-4B1A-976B-F138EE1E83BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E216ABE0-7DAB-4029-A91C-64BD31297568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="1280" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Rest!$B$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="206">
   <si>
     <t>Part Number</t>
   </si>
@@ -1766,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,9 +3204,7 @@
       <c r="D38" t="s">
         <v>156</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="F38" s="4"/>
       <c r="G38" s="27" t="s">
         <v>157</v>
       </c>

</xml_diff>